<commit_message>
changed w and h carousel
</commit_message>
<xml_diff>
--- a/frontend/data/wasteitemsexcel.xlsx
+++ b/frontend/data/wasteitemsexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\KUL\Thesis\data_waste_collection_app\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787D1CBA-8F15-4D06-AAD1-D20AB45E71C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A57A115-4065-47B1-99CD-3B09F3E97C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>imgCount</t>
   </si>
   <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>name_en</t>
   </si>
   <si>
@@ -208,6 +205,12 @@
   </si>
   <si>
     <t>Dit is de tweede afbeelding</t>
+  </si>
+  <si>
+    <t>Don't know if it is recyclable? Click the image!</t>
+  </si>
+  <si>
+    <t>Niet zeker of het recycleerbaar is? Klik op de foto!</t>
   </si>
 </sst>
 </file>
@@ -574,31 +577,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB177D8D-0680-4D49-8ED2-39533DF946A1}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="31.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="11" width="13.21875" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" customWidth="1"/>
+    <col min="7" max="10" width="40.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -622,17 +625,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -640,38 +640,38 @@
         <f>COUNTIF(Content!B:B,A2)</f>
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -679,38 +679,38 @@
         <f>COUNTIF(Content!B:B,A3)</f>
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -718,38 +718,38 @@
         <f>COUNTIF(Content!B:B,A4)</f>
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -757,38 +757,38 @@
         <f>COUNTIF(Content!B:B,A5)</f>
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -796,26 +796,32 @@
         <f>COUNTIF(Content!B:B,A6)</f>
         <v>1</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -823,26 +829,26 @@
         <f>COUNTIF(Content!B:B,A7)</f>
         <v>1</v>
       </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" t="s">
-        <v>44</v>
+      <c r="K7">
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -850,26 +856,26 @@
         <f>COUNTIF(Content!B:B,A8)</f>
         <v>1</v>
       </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" t="s">
         <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
-        <v>44</v>
+      <c r="K8">
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -877,26 +883,26 @@
         <f>COUNTIF(Content!B:B,A9)</f>
         <v>1</v>
       </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="s">
-        <v>44</v>
+      <c r="K9">
+        <v>0</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -904,26 +910,26 @@
         <f>COUNTIF(Content!B:B,A10)</f>
         <v>1</v>
       </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>43</v>
       </c>
-      <c r="G10" t="s">
-        <v>44</v>
+      <c r="K10">
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -931,8 +937,11 @@
         <f>COUNTIF(Content!B:B,A11)</f>
         <v>1</v>
       </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -940,13 +949,10 @@
       <c r="F11" t="s">
         <v>43</v>
       </c>
-      <c r="G11" t="s">
-        <v>44</v>
+      <c r="K11">
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
         <v>0</v>
       </c>
     </row>
@@ -960,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207FEB07-A67A-4617-8B73-304D937D831E}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -976,22 +982,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1002,19 +1008,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1025,19 +1031,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>50</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>51</v>
-      </c>
-      <c r="G3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1048,19 +1054,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1071,19 +1077,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1094,19 +1100,19 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1117,19 +1123,19 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,19 +1146,19 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1163,19 +1169,19 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1186,19 +1192,19 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1209,19 +1215,19 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1232,19 +1238,19 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1255,19 +1261,19 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all translations now come from an excel
</commit_message>
<xml_diff>
--- a/frontend/data/wasteitemsexcel.xlsx
+++ b/frontend/data/wasteitemsexcel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\KUL\Thesis\data_waste_collection_app\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A57A115-4065-47B1-99CD-3B09F3E97C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FDD346-6A52-4D56-BA71-32A9DA743C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="Content" sheetId="2" r:id="rId2"/>
+    <sheet name="Messages" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -211,6 +212,153 @@
   </si>
   <si>
     <t>Niet zeker of het recycleerbaar is? Klik op de foto!</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>aw</t>
+  </si>
+  <si>
+    <t>toolbarTitle</t>
+  </si>
+  <si>
+    <t>listTitle</t>
+  </si>
+  <si>
+    <t>loadingText</t>
+  </si>
+  <si>
+    <t>submitButton</t>
+  </si>
+  <si>
+    <t>What did you throw away?</t>
+  </si>
+  <si>
+    <t>Let's collect data!</t>
+  </si>
+  <si>
+    <t>Loading application...</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Laten we data verzamelen!</t>
+  </si>
+  <si>
+    <t>Wat heeft u weggegooid?</t>
+  </si>
+  <si>
+    <t>Verstuur</t>
+  </si>
+  <si>
+    <t>defaultThankYouMessage</t>
+  </si>
+  <si>
+    <t>co2MessagePart1</t>
+  </si>
+  <si>
+    <t>co2MessagePart2</t>
+  </si>
+  <si>
+    <t>askFeedback</t>
+  </si>
+  <si>
+    <t>clickHere</t>
+  </si>
+  <si>
+    <t>normalBin</t>
+  </si>
+  <si>
+    <t>Thank you for registering your waste!</t>
+  </si>
+  <si>
+    <t>This recycle bin already saved</t>
+  </si>
+  <si>
+    <t>kg of CO2!</t>
+  </si>
+  <si>
+    <t>Would you be so kind to give some feedback on the app?</t>
+  </si>
+  <si>
+    <t>Click here</t>
+  </si>
+  <si>
+    <t>Normal bin</t>
+  </si>
+  <si>
+    <t>Applicatie aan het laden...</t>
+  </si>
+  <si>
+    <t>Bedankt om uw afval te registreren!</t>
+  </si>
+  <si>
+    <t>Deze vuilbak heeft al</t>
+  </si>
+  <si>
+    <t>kg CO2 bespaard!</t>
+  </si>
+  <si>
+    <t>Zou u aub wat feedback willen geven over de app?</t>
+  </si>
+  <si>
+    <t>Klik hier</t>
+  </si>
+  <si>
+    <t>Normale vuilbak</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>Papiamento!</t>
+  </si>
+  <si>
+    <t>Español!</t>
+  </si>
+  <si>
+    <t>recyclingBin</t>
+  </si>
+  <si>
+    <t>nonRecyclingBin</t>
+  </si>
+  <si>
+    <t>hasToBeRecyclingBin</t>
+  </si>
+  <si>
+    <t>hasToBeNonRecyclingBin</t>
+  </si>
+  <si>
+    <t>Recycling bin</t>
+  </si>
+  <si>
+    <t>Non-recycling bin</t>
+  </si>
+  <si>
+    <t>This item belongs in the recycling bin</t>
+  </si>
+  <si>
+    <t>This item belongs in the non-recycling bin</t>
+  </si>
+  <si>
+    <t>Recyclingvuilbak</t>
+  </si>
+  <si>
+    <t>Niet-recyclingvuilbak</t>
+  </si>
+  <si>
+    <t>Dit item behoort in de recyclingvuilbak</t>
+  </si>
+  <si>
+    <t>Dit item behoort in de niet-recyclingvuilbak</t>
   </si>
 </sst>
 </file>
@@ -579,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB177D8D-0680-4D49-8ED2-39533DF946A1}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -967,7 +1115,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,24 +1430,269 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cd9202a6-e211-4275-8e27-b09f1131300c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444BD956-8AE9-416D-A362-3A03BEABFA02}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="4" width="30.5546875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="11" width="37.21875" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
+    <col min="13" max="13" width="23.21875" customWidth="1"/>
+    <col min="14" max="14" width="34.88671875" customWidth="1"/>
+    <col min="15" max="15" width="38" customWidth="1"/>
+    <col min="16" max="16" width="23.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" t="s">
+        <v>103</v>
+      </c>
+      <c r="M5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100371174F9DAA68943A4F64D1C7FA5190F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4f3fe012b06e40ce9d5bc16e3e412a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd9202a6-e211-4275-8e27-b09f1131300c" xmlns:ns4="61dace89-6e26-49db-a801-3b0b4dff7cd3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="526ac9343ee1d1ddb35fdc31bf83d2e3" ns3:_="" ns4:_="">
     <xsd:import namespace="cd9202a6-e211-4275-8e27-b09f1131300c"/>
@@ -1490,32 +1883,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FEF2F89-7996-4971-8EDE-6D5F154A3C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cd9202a6-e211-4275-8e27-b09f1131300c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="61dace89-6e26-49db-a801-3b0b4dff7cd3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7472511-D9E6-484D-AD19-CFCD51FA7DA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cd9202a6-e211-4275-8e27-b09f1131300c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA9E4F48-BA33-4883-999F-8D8FBDB5FA64}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1532,4 +1917,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7472511-D9E6-484D-AD19-CFCD51FA7DA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FEF2F89-7996-4971-8EDE-6D5F154A3C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cd9202a6-e211-4275-8e27-b09f1131300c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="61dace89-6e26-49db-a801-3b0b4dff7cd3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added 'more info' subtitle
</commit_message>
<xml_diff>
--- a/frontend/data/wasteitemsexcel.xlsx
+++ b/frontend/data/wasteitemsexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\KUL\Thesis\data_waste_collection_app\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FDD346-6A52-4D56-BA71-32A9DA743C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB39F7E5-6117-404D-82DF-D7D5486F14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>Dit item behoort in de niet-recyclingvuilbak</t>
+  </si>
+  <si>
+    <t>To get more information about an item, press the picture!</t>
+  </si>
+  <si>
+    <t>moreInformationPressPicture</t>
+  </si>
+  <si>
+    <t>Om meer info te krijgen over een item, druk op de foto!</t>
   </si>
 </sst>
 </file>
@@ -1432,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444BD956-8AE9-416D-A362-3A03BEABFA02}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,10 +1457,10 @@
     <col min="13" max="13" width="23.21875" customWidth="1"/>
     <col min="14" max="14" width="34.88671875" customWidth="1"/>
     <col min="15" max="15" width="38" customWidth="1"/>
-    <col min="16" max="16" width="23.21875" customWidth="1"/>
+    <col min="16" max="16" width="51.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -1497,8 +1506,11 @@
       <c r="O1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1544,8 +1556,11 @@
       <c r="O2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1591,8 +1606,11 @@
       <c r="O3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1638,8 +1656,11 @@
       <c r="O4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1684,6 +1705,9 @@
       </c>
       <c r="O5" t="s">
         <v>106</v>
+      </c>
+      <c r="P5" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1693,6 +1717,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100371174F9DAA68943A4F64D1C7FA5190F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4f3fe012b06e40ce9d5bc16e3e412a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd9202a6-e211-4275-8e27-b09f1131300c" xmlns:ns4="61dace89-6e26-49db-a801-3b0b4dff7cd3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="526ac9343ee1d1ddb35fdc31bf83d2e3" ns3:_="" ns4:_="">
     <xsd:import namespace="cd9202a6-e211-4275-8e27-b09f1131300c"/>
@@ -1883,15 +1916,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1901,6 +1925,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7472511-D9E6-484D-AD19-CFCD51FA7DA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA9E4F48-BA33-4883-999F-8D8FBDB5FA64}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1915,14 +1947,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7472511-D9E6-484D-AD19-CFCD51FA7DA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
pwa precaching + animatedCounter
</commit_message>
<xml_diff>
--- a/frontend/data/wasteitemsexcel.xlsx
+++ b/frontend/data/wasteitemsexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\KUL\Thesis\data_waste_collection_app\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB39F7E5-6117-404D-82DF-D7D5486F14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37891D56-F61F-4DAB-B496-1FFCC5175E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{C9F1FE1B-63EA-4E9A-B67A-DB8A9DD9CABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -1124,7 +1124,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,16 +1144,16 @@
       <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1436,15 +1436,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444BD956-8AE9-416D-A362-3A03BEABFA02}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,57 +1461,60 @@
     <col min="16" max="16" width="51.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1610,7 +1614,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1660,7 +1664,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1717,15 +1721,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100371174F9DAA68943A4F64D1C7FA5190F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4f3fe012b06e40ce9d5bc16e3e412a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd9202a6-e211-4275-8e27-b09f1131300c" xmlns:ns4="61dace89-6e26-49db-a801-3b0b4dff7cd3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="526ac9343ee1d1ddb35fdc31bf83d2e3" ns3:_="" ns4:_="">
     <xsd:import namespace="cd9202a6-e211-4275-8e27-b09f1131300c"/>
@@ -1916,6 +1911,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1925,14 +1929,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7472511-D9E6-484D-AD19-CFCD51FA7DA3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA9E4F48-BA33-4883-999F-8D8FBDB5FA64}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1947,6 +1943,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7472511-D9E6-484D-AD19-CFCD51FA7DA3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>